<commit_message>
Modificaciones del 13 de julio en el Tec
</commit_message>
<xml_diff>
--- a/produccion_lineas.xlsx
+++ b/produccion_lineas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S2G 02\Desktop\FEMSUKI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisc\OneDrive\Documentos\GitHub\Project1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9E5E40E5-AD67-49BA-8AF0-6602FB6ABBE6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="8_{9E5E40E5-AD67-49BA-8AF0-6602FB6ABBE6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{1A7DE6F3-2D36-4432-B30A-6B26737ABA6E}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="27870" windowHeight="12810" xr2:uid="{EBEFC286-A746-455B-ABCC-CE2682BAA240}"/>
+    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{EBEFC286-A746-455B-ABCC-CE2682BAA240}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -32,21 +32,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="217">
   <si>
-    <t>Fecha FEMSA</t>
-  </si>
-  <si>
-    <t>Prod. Linea 1</t>
-  </si>
-  <si>
-    <t>Prod. Linea 2</t>
-  </si>
-  <si>
-    <t>Prod. Linea 3</t>
-  </si>
-  <si>
-    <t>Prod. Linea 4</t>
-  </si>
-  <si>
     <t>31/07/2019</t>
   </si>
   <si>
@@ -681,6 +666,21 @@
   </si>
   <si>
     <t>01/01/2019</t>
+  </si>
+  <si>
+    <t>Fecha</t>
+  </si>
+  <si>
+    <t>Prod. Linea 1(LTS)</t>
+  </si>
+  <si>
+    <t>Prod. Linea 2(LTS)</t>
+  </si>
+  <si>
+    <t>Prod. Linea 3(LTS)</t>
+  </si>
+  <si>
+    <t>Prod. Linea 4(LTS)</t>
   </si>
 </sst>
 </file>
@@ -743,7 +743,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1042,374 +1042,375 @@
   <dimension ref="A1:E213"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>212</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1">
-        <v>0</v>
-      </c>
-      <c r="E2" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0</v>
-      </c>
-      <c r="E3" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="B8" s="1">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="1">
-        <v>0</v>
-      </c>
-      <c r="C4" s="1">
-        <v>0</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1">
-        <v>0</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="B10" s="1">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="1">
-        <v>0</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0</v>
-      </c>
-      <c r="E6" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="B11" s="1">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="1">
-        <v>0</v>
-      </c>
-      <c r="C7" s="1">
-        <v>0</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0</v>
-      </c>
-      <c r="E7" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="B12" s="1">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="1">
-        <v>0</v>
-      </c>
-      <c r="C8" s="1">
-        <v>0</v>
-      </c>
-      <c r="D8" s="1">
-        <v>0</v>
-      </c>
-      <c r="E8" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="B13" s="1">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="1">
-        <v>0</v>
-      </c>
-      <c r="C9" s="1">
-        <v>0</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0</v>
-      </c>
-      <c r="E9" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="B14" s="1">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="1">
-        <v>0</v>
-      </c>
-      <c r="C10" s="1">
-        <v>0</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0</v>
-      </c>
-      <c r="E10" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="B15" s="1">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="1">
-        <v>0</v>
-      </c>
-      <c r="C11" s="1">
-        <v>0</v>
-      </c>
-      <c r="D11" s="1">
-        <v>0</v>
-      </c>
-      <c r="E11" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="B16" s="1">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="1">
-        <v>0</v>
-      </c>
-      <c r="C12" s="1">
-        <v>0</v>
-      </c>
-      <c r="D12" s="1">
-        <v>0</v>
-      </c>
-      <c r="E12" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="B17" s="1">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="1">
-        <v>0</v>
-      </c>
-      <c r="C13" s="1">
-        <v>0</v>
-      </c>
-      <c r="D13" s="1">
-        <v>0</v>
-      </c>
-      <c r="E13" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="B18" s="1">
+        <v>0</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="1">
-        <v>0</v>
-      </c>
-      <c r="C14" s="1">
-        <v>0</v>
-      </c>
-      <c r="D14" s="1">
-        <v>0</v>
-      </c>
-      <c r="E14" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="B19" s="1">
+        <v>0</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="1">
-        <v>0</v>
-      </c>
-      <c r="C15" s="1">
-        <v>0</v>
-      </c>
-      <c r="D15" s="1">
-        <v>0</v>
-      </c>
-      <c r="E15" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="B20" s="1">
+        <v>0</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="1">
-        <v>0</v>
-      </c>
-      <c r="C16" s="1">
-        <v>0</v>
-      </c>
-      <c r="D16" s="1">
-        <v>0</v>
-      </c>
-      <c r="E16" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="B21" s="1">
+        <v>0</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="B17" s="1">
-        <v>0</v>
-      </c>
-      <c r="C17" s="1">
-        <v>0</v>
-      </c>
-      <c r="D17" s="1">
-        <v>0</v>
-      </c>
-      <c r="E17" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="1">
-        <v>0</v>
-      </c>
-      <c r="C18" s="1">
-        <v>0</v>
-      </c>
-      <c r="D18" s="1">
-        <v>0</v>
-      </c>
-      <c r="E18" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" s="1">
-        <v>0</v>
-      </c>
-      <c r="C19" s="1">
-        <v>0</v>
-      </c>
-      <c r="D19" s="1">
-        <v>0</v>
-      </c>
-      <c r="E19" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" s="1">
-        <v>0</v>
-      </c>
-      <c r="C20" s="1">
-        <v>0</v>
-      </c>
-      <c r="D20" s="1">
-        <v>0</v>
-      </c>
-      <c r="E20" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" s="1">
-        <v>0</v>
-      </c>
-      <c r="C21" s="1">
-        <v>0</v>
-      </c>
-      <c r="D21" s="1">
-        <v>0</v>
-      </c>
-      <c r="E21" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="B22" s="1">
         <v>583200</v>
@@ -1424,9 +1425,9 @@
         <v>1153440</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B23" s="1">
         <v>739872</v>
@@ -1441,9 +1442,9 @@
         <v>491184</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B24" s="1">
         <v>626368</v>
@@ -1458,9 +1459,9 @@
         <v>1004400</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B25" s="1">
         <v>516640</v>
@@ -1475,9 +1476,9 @@
         <v>1156680</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B26" s="1">
         <v>608800</v>
@@ -1492,9 +1493,9 @@
         <v>537192</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B27" s="1">
         <v>1087488</v>
@@ -1509,9 +1510,9 @@
         <v>811296</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B28" s="1">
         <v>301056</v>
@@ -1526,9 +1527,9 @@
         <v>955152</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B29" s="1">
         <v>0</v>
@@ -1543,9 +1544,9 @@
         <v>1147608</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B30" s="1">
         <v>0</v>
@@ -1560,9 +1561,9 @@
         <v>493128</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B31" s="1">
         <v>0</v>
@@ -1577,9 +1578,9 @@
         <v>1175472</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B32" s="1">
         <v>0</v>
@@ -1594,9 +1595,9 @@
         <v>952560</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B33" s="1">
         <v>1005312</v>
@@ -1611,9 +1612,9 @@
         <v>1144368</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B34" s="1">
         <v>808000</v>
@@ -1628,9 +1629,9 @@
         <v>1148256</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B35" s="1">
         <v>496608</v>
@@ -1645,9 +1646,9 @@
         <v>743904</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B36" s="1">
         <v>807168</v>
@@ -1662,9 +1663,9 @@
         <v>899424</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B37" s="1">
         <v>1080480</v>
@@ -1679,9 +1680,9 @@
         <v>884520</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B38" s="1">
         <v>533376</v>
@@ -1696,9 +1697,9 @@
         <v>651888</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B39" s="1">
         <v>832608</v>
@@ -1713,9 +1714,9 @@
         <v>942192</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B40" s="1">
         <v>995552</v>
@@ -1730,9 +1731,9 @@
         <v>1118448</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B41" s="1">
         <v>710528</v>
@@ -1747,9 +1748,9 @@
         <v>956448</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B42" s="1">
         <v>1178112</v>
@@ -1764,9 +1765,9 @@
         <v>1146960</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B43" s="1">
         <v>694048</v>
@@ -1781,9 +1782,9 @@
         <v>1110672</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B44" s="1">
         <v>670544</v>
@@ -1798,9 +1799,9 @@
         <v>343440</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B45" s="1">
         <v>489216</v>
@@ -1815,9 +1816,9 @@
         <v>932472</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B46" s="1">
         <v>1163520</v>
@@ -1832,9 +1833,9 @@
         <v>515808</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B47" s="1">
         <v>1072768</v>
@@ -1849,9 +1850,9 @@
         <v>771120</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B48" s="1">
         <v>643776</v>
@@ -1866,9 +1867,9 @@
         <v>1049760</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B49" s="1">
         <v>602632</v>
@@ -1883,9 +1884,9 @@
         <v>849528</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B50" s="1">
         <v>988704</v>
@@ -1900,9 +1901,9 @@
         <v>1132704</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B51" s="1">
         <v>741376</v>
@@ -1917,9 +1918,9 @@
         <v>911088</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B52" s="1">
         <v>252160</v>
@@ -1934,9 +1935,9 @@
         <v>992736</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B53" s="1">
         <v>726320</v>
@@ -1951,9 +1952,9 @@
         <v>190512</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B54" s="1">
         <v>844880</v>
@@ -1968,9 +1969,9 @@
         <v>968112</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B55" s="1">
         <v>765696</v>
@@ -1985,9 +1986,9 @@
         <v>1139832</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B56" s="1">
         <v>801792</v>
@@ -2002,9 +2003,9 @@
         <v>1194912</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B57" s="1">
         <v>896256</v>
@@ -2019,9 +2020,9 @@
         <v>1028376</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B58" s="1">
         <v>797680</v>
@@ -2036,9 +2037,9 @@
         <v>45360</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B59" s="1">
         <v>228480</v>
@@ -2053,9 +2054,9 @@
         <v>1119744</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B60" s="1">
         <v>1069824</v>
@@ -2070,9 +2071,9 @@
         <v>965520</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B61" s="1">
         <v>671088</v>
@@ -2087,9 +2088,9 @@
         <v>1069200</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B62" s="1">
         <v>754240</v>
@@ -2104,9 +2105,9 @@
         <v>984960</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B63" s="1">
         <v>785280</v>
@@ -2121,9 +2122,9 @@
         <v>1132704</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B64" s="1">
         <v>850176</v>
@@ -2138,9 +2139,9 @@
         <v>1149552</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B65" s="1">
         <v>1178112</v>
@@ -2155,9 +2156,9 @@
         <v>463320</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B66" s="1">
         <v>390912</v>
@@ -2172,9 +2173,9 @@
         <v>1119744</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B67" s="1">
         <v>754400</v>
@@ -2189,9 +2190,9 @@
         <v>646056</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B68" s="1">
         <v>829920</v>
@@ -2206,9 +2207,9 @@
         <v>1163808</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B69" s="1">
         <v>627456</v>
@@ -2223,9 +2224,9 @@
         <v>978480</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B70" s="1">
         <v>949248</v>
@@ -2240,9 +2241,9 @@
         <v>1153440</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B71" s="1">
         <v>943456</v>
@@ -2257,9 +2258,9 @@
         <v>1132704</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B72" s="1">
         <v>499520</v>
@@ -2274,9 +2275,9 @@
         <v>226800</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B73" s="1">
         <v>496960</v>
@@ -2291,9 +2292,9 @@
         <v>1202688</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B74" s="1">
         <v>1013472</v>
@@ -2308,9 +2309,9 @@
         <v>1166400</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B75" s="1">
         <v>840192</v>
@@ -2325,9 +2326,9 @@
         <v>1109376</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B76" s="1">
         <v>847392</v>
@@ -2342,9 +2343,9 @@
         <v>1008936</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B77" s="1">
         <v>543712</v>
@@ -2359,9 +2360,9 @@
         <v>965520</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B78" s="1">
         <v>1097984</v>
@@ -2376,9 +2377,9 @@
         <v>1117800</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B79" s="1">
         <v>612864</v>
@@ -2393,9 +2394,9 @@
         <v>372600</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B80" s="1">
         <v>468000</v>
@@ -2410,9 +2411,9 @@
         <v>1115856</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B81" s="1">
         <v>972032</v>
@@ -2427,9 +2428,9 @@
         <v>811296</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B82" s="1">
         <v>856064</v>
@@ -2444,9 +2445,9 @@
         <v>1031616</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B83" s="1">
         <v>576256</v>
@@ -2461,9 +2462,9 @@
         <v>1117152</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B84" s="1">
         <v>613320</v>
@@ -2478,9 +2479,9 @@
         <v>1021248</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B85" s="1">
         <v>935584</v>
@@ -2495,9 +2496,9 @@
         <v>987552</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B86" s="1">
         <v>990800</v>
@@ -2512,9 +2513,9 @@
         <v>247536</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B87" s="1">
         <v>357760</v>
@@ -2529,9 +2530,9 @@
         <v>1043928</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B88" s="1">
         <v>975872</v>
@@ -2546,9 +2547,9 @@
         <v>312336</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B89" s="1">
         <v>618240</v>
@@ -2563,9 +2564,9 @@
         <v>1168992</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B90" s="1">
         <v>885504</v>
@@ -2580,9 +2581,9 @@
         <v>822960</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B91" s="1">
         <v>682104</v>
@@ -2597,9 +2598,9 @@
         <v>1166400</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B92" s="1">
         <v>696400</v>
@@ -2614,9 +2615,9 @@
         <v>1130112</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B93" s="1">
         <v>895488</v>
@@ -2631,9 +2632,9 @@
         <v>371304</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B94" s="1">
         <v>459840</v>
@@ -2648,9 +2649,9 @@
         <v>1115856</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B95" s="1">
         <v>484560</v>
@@ -2665,9 +2666,9 @@
         <v>1145664</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B96" s="1">
         <v>796352</v>
@@ -2682,9 +2683,9 @@
         <v>1143072</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B97" s="1">
         <v>854672</v>
@@ -2699,9 +2700,9 @@
         <v>1000512</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B98" s="1">
         <v>632080</v>
@@ -2716,9 +2717,9 @@
         <v>1126224</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B99" s="1">
         <v>784896</v>
@@ -2733,9 +2734,9 @@
         <v>1104840</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B100" s="1">
         <v>899968</v>
@@ -2750,9 +2751,9 @@
         <v>544320</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B101" s="1">
         <v>357440</v>
@@ -2767,9 +2768,9 @@
         <v>1044576</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B102" s="1">
         <v>535040</v>
@@ -2784,9 +2785,9 @@
         <v>194400</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B103" s="1">
         <v>916800</v>
@@ -2801,9 +2802,9 @@
         <v>763344</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B104" s="1">
         <v>869376</v>
@@ -2818,9 +2819,9 @@
         <v>832032</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B105" s="1">
         <v>0</v>
@@ -2835,9 +2836,9 @@
         <v>1131408</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B106" s="1">
         <v>881664</v>
@@ -2852,9 +2853,9 @@
         <v>1110672</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B107" s="1">
         <v>777312</v>
@@ -2869,9 +2870,9 @@
         <v>771120</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B108" s="1">
         <v>346112</v>
@@ -2886,9 +2887,9 @@
         <v>1130112</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B109" s="1">
         <v>1229568</v>
@@ -2903,9 +2904,9 @@
         <v>1083456</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B110" s="1">
         <v>930688</v>
@@ -2920,9 +2921,9 @@
         <v>1041984</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B111" s="1">
         <v>620672</v>
@@ -2937,9 +2938,9 @@
         <v>1080864</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B112" s="1">
         <v>544000</v>
@@ -2954,9 +2955,9 @@
         <v>1140480</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B113" s="1">
         <v>1082880</v>
@@ -2971,9 +2972,9 @@
         <v>1117152</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B114" s="1">
         <v>744384</v>
@@ -2988,9 +2989,9 @@
         <v>263088</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B115" s="1">
         <v>0</v>
@@ -3005,9 +3006,9 @@
         <v>1025784</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B116" s="1">
         <v>871328</v>
@@ -3022,9 +3023,9 @@
         <v>1054944</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B117" s="1">
         <v>507680</v>
@@ -3039,9 +3040,9 @@
         <v>1096416</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B118" s="1">
         <v>410240</v>
@@ -3056,9 +3057,9 @@
         <v>939600</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B119" s="1">
         <v>446880</v>
@@ -3073,9 +3074,9 @@
         <v>1093824</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B120" s="1">
         <v>609024</v>
@@ -3090,9 +3091,9 @@
         <v>1126224</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B121" s="1">
         <v>496128</v>
@@ -3107,9 +3108,9 @@
         <v>263088</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B122" s="1">
         <v>426240</v>
@@ -3124,9 +3125,9 @@
         <v>554040</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B123" s="1">
         <v>797340</v>
@@ -3141,9 +3142,9 @@
         <v>1118448</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B124" s="1">
         <v>1056768</v>
@@ -3158,9 +3159,9 @@
         <v>974592</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B125" s="1">
         <v>634368</v>
@@ -3175,9 +3176,9 @@
         <v>1037448</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B126" s="1">
         <v>417600</v>
@@ -3192,9 +3193,9 @@
         <v>1082808</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B127" s="1">
         <v>598368</v>
@@ -3209,9 +3210,9 @@
         <v>1143072</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B128" s="1">
         <v>638208</v>
@@ -3226,9 +3227,9 @@
         <v>421848</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B129" s="1">
         <v>362880</v>
@@ -3243,9 +3244,9 @@
         <v>1174176</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B130" s="1">
         <v>788224</v>
@@ -3260,9 +3261,9 @@
         <v>1121040</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B131" s="1">
         <v>812256</v>
@@ -3277,9 +3278,9 @@
         <v>1071144</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B132" s="1">
         <v>442400</v>
@@ -3294,9 +3295,9 @@
         <v>983016</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B133" s="1">
         <v>423168</v>
@@ -3311,9 +3312,9 @@
         <v>1163808</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B134" s="1">
         <v>1119744</v>
@@ -3328,9 +3329,9 @@
         <v>1154736</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135" s="1" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B135" s="1">
         <v>547780</v>
@@ -3345,9 +3346,9 @@
         <v>295488</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B136" s="1">
         <v>328500</v>
@@ -3362,9 +3363,9 @@
         <v>843696</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B137" s="1">
         <v>0</v>
@@ -3379,9 +3380,9 @@
         <v>929232</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" s="1" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B138" s="1">
         <v>1216512</v>
@@ -3396,9 +3397,9 @@
         <v>1150848</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B139" s="1">
         <v>667200</v>
@@ -3413,9 +3414,9 @@
         <v>1166400</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="B140" s="1">
         <v>619008</v>
@@ -3430,9 +3431,9 @@
         <v>968112</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" s="1" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B141" s="1">
         <v>954624</v>
@@ -3447,9 +3448,9 @@
         <v>1179360</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B142" s="1">
         <v>594656</v>
@@ -3464,9 +3465,9 @@
         <v>1146960</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B143" s="1">
         <v>497984</v>
@@ -3481,9 +3482,9 @@
         <v>1044576</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B144" s="1">
         <v>1217280</v>
@@ -3498,9 +3499,9 @@
         <v>469152</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B145" s="1">
         <v>850944</v>
@@ -3515,9 +3516,9 @@
         <v>1145664</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B146" s="1">
         <v>563104</v>
@@ -3532,9 +3533,9 @@
         <v>1110672</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" s="1" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B147" s="1">
         <v>804480</v>
@@ -3549,9 +3550,9 @@
         <v>988848</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B148" s="1">
         <v>642816</v>
@@ -3566,9 +3567,9 @@
         <v>1008936</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" s="1" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B149" s="1">
         <v>561280</v>
@@ -3583,9 +3584,9 @@
         <v>817776</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" s="1" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B150" s="1">
         <v>550912</v>
@@ -3600,9 +3601,9 @@
         <v>719280</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" s="1" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B151" s="1">
         <v>1092864</v>
@@ -3617,9 +3618,9 @@
         <v>1146960</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" s="1" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B152" s="1">
         <v>805600</v>
@@ -3634,9 +3635,9 @@
         <v>981072</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153" s="1" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B153" s="1">
         <v>942816</v>
@@ -3651,9 +3652,9 @@
         <v>1108728</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154" s="1" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B154" s="1">
         <v>433920</v>
@@ -3668,9 +3669,9 @@
         <v>1131408</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155" s="1" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B155" s="1">
         <v>1157376</v>
@@ -3685,9 +3686,9 @@
         <v>1100304</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156" s="1" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B156" s="1">
         <v>138240</v>
@@ -3702,9 +3703,9 @@
         <v>196992</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157" s="1" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="B157" s="1">
         <v>161920</v>
@@ -3719,9 +3720,9 @@
         <v>1142424</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158" s="1" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="B158" s="1">
         <v>799900</v>
@@ -3736,9 +3737,9 @@
         <v>829440</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A159" s="1" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B159" s="1">
         <v>854816</v>
@@ -3753,9 +3754,9 @@
         <v>1086048</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160" s="1" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="B160" s="1">
         <v>319488</v>
@@ -3770,9 +3771,9 @@
         <v>1146960</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A161" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="B161" s="1">
         <v>426240</v>
@@ -3787,9 +3788,9 @@
         <v>1014768</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162" s="1" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="B162" s="1">
         <v>963840</v>
@@ -3804,9 +3805,9 @@
         <v>905904</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A163" s="1" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B163" s="1">
         <v>991488</v>
@@ -3821,9 +3822,9 @@
         <v>1118448</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A164" s="1" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B164" s="1">
         <v>0</v>
@@ -3838,9 +3839,9 @@
         <v>1062720</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165" s="1" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B165" s="1">
         <v>939456</v>
@@ -3855,9 +3856,9 @@
         <v>542376</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166" s="1" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B166" s="1">
         <v>513600</v>
@@ -3872,9 +3873,9 @@
         <v>1124928</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167" s="1" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B167" s="1">
         <v>586752</v>
@@ -3889,9 +3890,9 @@
         <v>1137888</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168" s="1" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="B168" s="1">
         <v>622848</v>
@@ -3906,9 +3907,9 @@
         <v>1001808</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169" s="1" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B169" s="1">
         <v>1256448</v>
@@ -3923,9 +3924,9 @@
         <v>905256</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170" s="1" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="B170" s="1">
         <v>686208</v>
@@ -3940,9 +3941,9 @@
         <v>1043928</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A171" s="1" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B171" s="1">
         <v>41600</v>
@@ -3957,9 +3958,9 @@
         <v>1121688</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A172" s="1" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="B172" s="1">
         <v>566400</v>
@@ -3974,9 +3975,9 @@
         <v>203472</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A173" s="1" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="B173" s="1">
         <v>694272</v>
@@ -3991,9 +3992,9 @@
         <v>755568</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A174" s="1" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="B174" s="1">
         <v>666112</v>
@@ -4008,9 +4009,9 @@
         <v>1136592</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A175" s="1" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B175" s="1">
         <v>909440</v>
@@ -4025,9 +4026,9 @@
         <v>1143072</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A176" s="1" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="B176" s="1">
         <v>1023744</v>
@@ -4042,9 +4043,9 @@
         <v>909144</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A177" s="1" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B177" s="1">
         <v>983744</v>
@@ -4059,9 +4060,9 @@
         <v>1056240</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A178" s="1" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="B178" s="1">
         <v>284400</v>
@@ -4076,9 +4077,9 @@
         <v>1000512</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A179" s="1" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="B179" s="1">
         <v>0</v>
@@ -4093,9 +4094,9 @@
         <v>537840</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A180" s="1" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B180" s="1">
         <v>159744</v>
@@ -4110,9 +4111,9 @@
         <v>1108080</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A181" s="1" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="B181" s="1">
         <v>698112</v>
@@ -4127,9 +4128,9 @@
         <v>957744</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A182" s="1" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="B182" s="1">
         <v>822528</v>
@@ -4144,9 +4145,9 @@
         <v>1098360</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A183" s="1" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="B183" s="1">
         <v>475392</v>
@@ -4161,9 +4162,9 @@
         <v>1158624</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A184" s="1" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="B184" s="1">
         <v>593600</v>
@@ -4178,9 +4179,9 @@
         <v>601992</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A185" s="1" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="B185" s="1">
         <v>540672</v>
@@ -4195,9 +4196,9 @@
         <v>1122336</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A186" s="1" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B186" s="1">
         <v>1246464</v>
@@ -4212,9 +4213,9 @@
         <v>1101600</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A187" s="1" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="B187" s="1">
         <v>0</v>
@@ -4229,9 +4230,9 @@
         <v>773712</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A188" s="1" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B188" s="1">
         <v>53760</v>
@@ -4246,9 +4247,9 @@
         <v>1158624</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A189" s="1" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="B189" s="1">
         <v>1051392</v>
@@ -4263,9 +4264,9 @@
         <v>1123632</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A190" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="B190" s="1">
         <v>859264</v>
@@ -4280,9 +4281,9 @@
         <v>718632</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A191" s="1" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B191" s="1">
         <v>772480</v>
@@ -4297,9 +4298,9 @@
         <v>1076328</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A192" s="1" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="B192" s="1">
         <v>262656</v>
@@ -4314,9 +4315,9 @@
         <v>1109376</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A193" s="1" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="B193" s="1">
         <v>152832</v>
@@ -4331,9 +4332,9 @@
         <v>1091232</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A194" s="1" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="B194" s="1">
         <v>0</v>
@@ -4348,9 +4349,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A195" s="1" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="B195" s="1">
         <v>0</v>
@@ -4365,9 +4366,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A196" s="1" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="B196" s="1">
         <v>0</v>
@@ -4382,9 +4383,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A197" s="1" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="B197" s="1">
         <v>1067520</v>
@@ -4399,9 +4400,9 @@
         <v>1153440</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A198" s="1" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="B198" s="1">
         <v>906784</v>
@@ -4416,9 +4417,9 @@
         <v>1174176</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A199" s="1" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B199" s="1">
         <v>0</v>
@@ -4433,9 +4434,9 @@
         <v>970704</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A200" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B200" s="1">
         <v>901632</v>
@@ -4450,9 +4451,9 @@
         <v>1168992</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A201" s="1" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B201" s="1">
         <v>473088</v>
@@ -4467,9 +4468,9 @@
         <v>1127520</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A202" s="1" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B202" s="1">
         <v>963552</v>
@@ -4484,9 +4485,9 @@
         <v>847584</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A203" s="1" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="B203" s="1">
         <v>362400</v>
@@ -4501,9 +4502,9 @@
         <v>1183248</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A204" s="1" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="B204" s="1">
         <v>949248</v>
@@ -4518,9 +4519,9 @@
         <v>1140480</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A205" s="1" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="B205" s="1">
         <v>600192</v>
@@ -4535,9 +4536,9 @@
         <v>946080</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A206" s="1" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="B206" s="1">
         <v>0</v>
@@ -4552,9 +4553,9 @@
         <v>1101600</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A207" s="1" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="B207" s="1">
         <v>631680</v>
@@ -4569,9 +4570,9 @@
         <v>1136592</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A208" s="1" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="B208" s="1">
         <v>916992</v>
@@ -4586,9 +4587,9 @@
         <v>393984</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A209" s="1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B209" s="1">
         <v>442880</v>
@@ -4603,9 +4604,9 @@
         <v>644112</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A210" s="1" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B210" s="1">
         <v>533504</v>
@@ -4620,9 +4621,9 @@
         <v>995328</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A211" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="B211" s="1">
         <v>1108224</v>
@@ -4637,9 +4638,9 @@
         <v>1114560</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A212" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="B212" s="1">
         <v>820448</v>
@@ -4654,9 +4655,9 @@
         <v>1150848</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A213" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="B213" s="1">
         <v>640512</v>

</xml_diff>